<commit_message>
Pruebas sobre guardado de archivos
</commit_message>
<xml_diff>
--- a/backend/uploads/Curso.xlsx
+++ b/backend/uploads/Curso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06f3652476c54f73/Escritorio/TFG/Datos/Asignaturas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06f3652476c54f73/Escritorio/Pruebas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_AD4DB114E441178AC67DF4B95E52FE28683EDF22" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBA9C3DC-4FC8-47B8-A186-498B0C67EB64}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_AD4DB114E441178AC67DF4B95E52FE28683EDF22" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D53803-D0FC-41B8-88B9-322EAD2028DA}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="15" windowWidth="20460" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="2190" windowWidth="26205" windowHeight="10770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <t>Curso</t>
   </si>
   <si>
-    <t>2024-25</t>
+    <t>2023-24</t>
   </si>
 </sst>
 </file>
@@ -99,10 +99,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,7 +367,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>